<commit_message>
recomienda ids de animes
</commit_message>
<xml_diff>
--- a/raw_data.xlsx
+++ b/raw_data.xlsx
@@ -799,7 +799,7 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>303.6</v>
+        <v>303.3</v>
       </c>
       <c r="D9" t="n">
         <v>5.95</v>
@@ -826,7 +826,7 @@
         <v>36</v>
       </c>
       <c r="L9" t="n">
-        <v>18213</v>
+        <v>18197</v>
       </c>
       <c r="M9" t="inlineStr"/>
     </row>
@@ -1467,16 +1467,16 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>172.9</v>
+        <v>172.3</v>
       </c>
       <c r="D25" t="n">
         <v>7.57</v>
       </c>
       <c r="E25" t="n">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="F25" t="n">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="G25" t="n">
         <v>28</v>
@@ -1485,16 +1485,16 @@
         <v>28</v>
       </c>
       <c r="I25" t="n">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="J25" t="n">
-        <v>984</v>
+        <v>978</v>
       </c>
       <c r="K25" t="n">
         <v>3</v>
       </c>
       <c r="L25" t="n">
-        <v>10419</v>
+        <v>10384</v>
       </c>
       <c r="M25" t="inlineStr">
         <is>
@@ -1813,19 +1813,19 @@
         </is>
       </c>
       <c r="O2" t="n">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="P2" t="n">
         <v>42</v>
       </c>
       <c r="Q2" t="n">
-        <v>86295</v>
+        <v>86255</v>
       </c>
       <c r="R2" t="n">
-        <v>1015015</v>
+        <v>1014558</v>
       </c>
       <c r="S2" t="n">
-        <v>1966181</v>
+        <v>1965187</v>
       </c>
       <c r="T2" t="inlineStr">
         <is>
@@ -1896,19 +1896,19 @@
         </is>
       </c>
       <c r="O3" t="n">
-        <v>210</v>
+        <v>216</v>
       </c>
       <c r="P3" t="n">
         <v>639</v>
       </c>
       <c r="Q3" t="n">
-        <v>1694</v>
+        <v>1695</v>
       </c>
       <c r="R3" t="n">
-        <v>224575</v>
+        <v>224491</v>
       </c>
       <c r="S3" t="n">
-        <v>396555</v>
+        <v>396379</v>
       </c>
       <c r="T3" t="inlineStr">
         <is>
@@ -1983,19 +1983,19 @@
         </is>
       </c>
       <c r="O4" t="n">
-        <v>370</v>
+        <v>377</v>
       </c>
       <c r="P4" t="n">
         <v>261</v>
       </c>
       <c r="Q4" t="n">
-        <v>16786</v>
+        <v>16780</v>
       </c>
       <c r="R4" t="n">
-        <v>387745</v>
+        <v>387605</v>
       </c>
       <c r="S4" t="n">
-        <v>800077</v>
+        <v>799739</v>
       </c>
       <c r="T4" t="inlineStr">
         <is>
@@ -2070,19 +2070,19 @@
         </is>
       </c>
       <c r="O5" t="n">
-        <v>3215</v>
+        <v>3176</v>
       </c>
       <c r="P5" t="n">
         <v>1942</v>
       </c>
       <c r="Q5" t="n">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="R5" t="n">
-        <v>45220</v>
+        <v>45203</v>
       </c>
       <c r="S5" t="n">
-        <v>122807</v>
+        <v>122688</v>
       </c>
       <c r="T5" t="inlineStr">
         <is>
@@ -2157,19 +2157,19 @@
         </is>
       </c>
       <c r="O6" t="n">
-        <v>4753</v>
+        <v>4726</v>
       </c>
       <c r="P6" t="n">
-        <v>5642</v>
+        <v>5638</v>
       </c>
       <c r="Q6" t="n">
         <v>16</v>
       </c>
       <c r="R6" t="n">
-        <v>6954</v>
+        <v>6953</v>
       </c>
       <c r="S6" t="n">
-        <v>16262</v>
+        <v>16260</v>
       </c>
       <c r="T6" t="inlineStr">
         <is>
@@ -2244,7 +2244,7 @@
         </is>
       </c>
       <c r="O7" t="n">
-        <v>810</v>
+        <v>814</v>
       </c>
       <c r="P7" t="n">
         <v>1361</v>
@@ -2253,10 +2253,10 @@
         <v>2067</v>
       </c>
       <c r="R7" t="n">
-        <v>91626</v>
+        <v>91608</v>
       </c>
       <c r="S7" t="n">
-        <v>190661</v>
+        <v>190549</v>
       </c>
       <c r="T7" t="inlineStr">
         <is>
@@ -2331,7 +2331,7 @@
         </is>
       </c>
       <c r="O8" t="n">
-        <v>702</v>
+        <v>697</v>
       </c>
       <c r="P8" t="n">
         <v>944</v>
@@ -2340,10 +2340,10 @@
         <v>4172</v>
       </c>
       <c r="R8" t="n">
-        <v>85567</v>
+        <v>85543</v>
       </c>
       <c r="S8" t="n">
-        <v>277575</v>
+        <v>277422</v>
       </c>
       <c r="T8" t="inlineStr">
         <is>
@@ -2418,19 +2418,19 @@
         </is>
       </c>
       <c r="O9" t="n">
-        <v>1841</v>
+        <v>1827</v>
       </c>
       <c r="P9" t="n">
-        <v>4671</v>
+        <v>4667</v>
       </c>
       <c r="Q9" t="n">
         <v>244</v>
       </c>
       <c r="R9" t="n">
-        <v>13923</v>
+        <v>13919</v>
       </c>
       <c r="S9" t="n">
-        <v>26156</v>
+        <v>26125</v>
       </c>
       <c r="T9" t="inlineStr">
         <is>
@@ -2505,19 +2505,19 @@
         </is>
       </c>
       <c r="O10" t="n">
-        <v>445</v>
+        <v>454</v>
       </c>
       <c r="P10" t="n">
-        <v>1279</v>
+        <v>1278</v>
       </c>
       <c r="Q10" t="n">
         <v>1388</v>
       </c>
       <c r="R10" t="n">
-        <v>113360</v>
+        <v>113308</v>
       </c>
       <c r="S10" t="n">
-        <v>203059</v>
+        <v>202876</v>
       </c>
       <c r="T10" t="inlineStr">
         <is>
@@ -2598,13 +2598,13 @@
         <v>122</v>
       </c>
       <c r="Q11" t="n">
-        <v>57568</v>
+        <v>57506</v>
       </c>
       <c r="R11" t="n">
-        <v>466402</v>
+        <v>465965</v>
       </c>
       <c r="S11" t="n">
-        <v>1228459</v>
+        <v>1227446</v>
       </c>
       <c r="T11" t="inlineStr">
         <is>
@@ -2679,19 +2679,19 @@
         </is>
       </c>
       <c r="O12" t="n">
-        <v>665</v>
+        <v>666</v>
       </c>
       <c r="P12" t="n">
         <v>9</v>
       </c>
       <c r="Q12" t="n">
-        <v>83001</v>
+        <v>82973</v>
       </c>
       <c r="R12" t="n">
-        <v>2056915</v>
+        <v>2056155</v>
       </c>
       <c r="S12" t="n">
-        <v>2986214</v>
+        <v>2984928</v>
       </c>
       <c r="T12" t="inlineStr">
         <is>
@@ -2766,19 +2766,19 @@
         </is>
       </c>
       <c r="O13" t="n">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="P13" t="n">
         <v>17</v>
       </c>
       <c r="Q13" t="n">
-        <v>237229</v>
+        <v>237054</v>
       </c>
       <c r="R13" t="n">
-        <v>1434888</v>
+        <v>1433761</v>
       </c>
       <c r="S13" t="n">
-        <v>2524779</v>
+        <v>2522600</v>
       </c>
       <c r="T13" t="inlineStr">
         <is>
@@ -2853,19 +2853,19 @@
         </is>
       </c>
       <c r="O14" t="n">
-        <v>936</v>
+        <v>945</v>
       </c>
       <c r="P14" t="n">
-        <v>1351</v>
+        <v>1350</v>
       </c>
       <c r="Q14" t="n">
         <v>3046</v>
       </c>
       <c r="R14" t="n">
-        <v>86921</v>
+        <v>86901</v>
       </c>
       <c r="S14" t="n">
-        <v>192092</v>
+        <v>191982</v>
       </c>
       <c r="T14" t="inlineStr">
         <is>
@@ -2943,16 +2943,16 @@
         <v>8021</v>
       </c>
       <c r="P15" t="n">
-        <v>8775</v>
+        <v>8769</v>
       </c>
       <c r="Q15" t="n">
         <v>3</v>
       </c>
       <c r="R15" t="n">
-        <v>1800</v>
+        <v>1799</v>
       </c>
       <c r="S15" t="n">
-        <v>5422</v>
+        <v>5423</v>
       </c>
       <c r="T15" t="inlineStr">
         <is>
@@ -3027,19 +3027,19 @@
         </is>
       </c>
       <c r="O16" t="n">
-        <v>868</v>
+        <v>877</v>
       </c>
       <c r="P16" t="n">
         <v>772</v>
       </c>
       <c r="Q16" t="n">
-        <v>5303</v>
+        <v>5301</v>
       </c>
       <c r="R16" t="n">
-        <v>152592</v>
+        <v>152563</v>
       </c>
       <c r="S16" t="n">
-        <v>337604</v>
+        <v>337409</v>
       </c>
       <c r="T16" t="inlineStr">
         <is>
@@ -3114,19 +3114,19 @@
         </is>
       </c>
       <c r="O17" t="n">
-        <v>2587</v>
+        <v>2550</v>
       </c>
       <c r="P17" t="n">
         <v>1695</v>
       </c>
       <c r="Q17" t="n">
-        <v>859</v>
+        <v>860</v>
       </c>
       <c r="R17" t="n">
-        <v>56872</v>
+        <v>56864</v>
       </c>
       <c r="S17" t="n">
-        <v>146304</v>
+        <v>146257</v>
       </c>
       <c r="T17" t="inlineStr">
         <is>
@@ -3201,7 +3201,7 @@
         </is>
       </c>
       <c r="O18" t="n">
-        <v>1183</v>
+        <v>1172</v>
       </c>
       <c r="P18" t="n">
         <v>975</v>
@@ -3210,10 +3210,10 @@
         <v>5351</v>
       </c>
       <c r="R18" t="n">
-        <v>60519</v>
+        <v>60486</v>
       </c>
       <c r="S18" t="n">
-        <v>269860</v>
+        <v>269599</v>
       </c>
       <c r="T18" t="inlineStr">
         <is>
@@ -3288,19 +3288,19 @@
         </is>
       </c>
       <c r="O19" t="n">
-        <v>2968</v>
+        <v>2986</v>
       </c>
       <c r="P19" t="n">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="Q19" t="n">
         <v>1379</v>
       </c>
       <c r="R19" t="n">
-        <v>82214</v>
+        <v>82208</v>
       </c>
       <c r="S19" t="n">
-        <v>192416</v>
+        <v>192365</v>
       </c>
       <c r="T19" t="inlineStr">
         <is>
@@ -3375,19 +3375,19 @@
         </is>
       </c>
       <c r="O20" t="n">
-        <v>815</v>
+        <v>819</v>
       </c>
       <c r="P20" t="n">
-        <v>2217</v>
+        <v>2218</v>
       </c>
       <c r="Q20" t="n">
         <v>928</v>
       </c>
       <c r="R20" t="n">
-        <v>42472</v>
+        <v>42462</v>
       </c>
       <c r="S20" t="n">
-        <v>102085</v>
+        <v>101995</v>
       </c>
       <c r="T20" t="inlineStr">
         <is>
@@ -3462,19 +3462,19 @@
         </is>
       </c>
       <c r="O21" t="n">
-        <v>2030</v>
+        <v>2045</v>
       </c>
       <c r="P21" t="n">
         <v>4810</v>
       </c>
       <c r="Q21" t="n">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="R21" t="n">
-        <v>8279</v>
+        <v>8273</v>
       </c>
       <c r="S21" t="n">
-        <v>24301</v>
+        <v>24288</v>
       </c>
       <c r="T21" t="inlineStr">
         <is>
@@ -3549,19 +3549,19 @@
         </is>
       </c>
       <c r="O22" t="n">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="P22" t="n">
         <v>45</v>
       </c>
       <c r="Q22" t="n">
-        <v>111746</v>
+        <v>111705</v>
       </c>
       <c r="R22" t="n">
-        <v>1149283</v>
+        <v>1148687</v>
       </c>
       <c r="S22" t="n">
-        <v>1922324</v>
+        <v>1921298</v>
       </c>
       <c r="T22" t="inlineStr">
         <is>
@@ -3632,7 +3632,7 @@
         </is>
       </c>
       <c r="O23" t="n">
-        <v>2075</v>
+        <v>2060</v>
       </c>
       <c r="P23" t="n">
         <v>964</v>
@@ -3641,10 +3641,10 @@
         <v>766</v>
       </c>
       <c r="R23" t="n">
-        <v>150633</v>
+        <v>150590</v>
       </c>
       <c r="S23" t="n">
-        <v>271802</v>
+        <v>271722</v>
       </c>
       <c r="T23" t="inlineStr">
         <is>
@@ -3715,19 +3715,19 @@
         </is>
       </c>
       <c r="O24" t="n">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="P24" t="n">
         <v>177</v>
       </c>
       <c r="Q24" t="n">
-        <v>30612</v>
+        <v>30599</v>
       </c>
       <c r="R24" t="n">
-        <v>658215</v>
+        <v>657898</v>
       </c>
       <c r="S24" t="n">
-        <v>986397</v>
+        <v>985843</v>
       </c>
       <c r="T24" t="inlineStr">
         <is>
@@ -3808,13 +3808,13 @@
         <v>302</v>
       </c>
       <c r="Q25" t="n">
-        <v>29794</v>
+        <v>29777</v>
       </c>
       <c r="R25" t="n">
-        <v>385173</v>
+        <v>384919</v>
       </c>
       <c r="S25" t="n">
-        <v>717128</v>
+        <v>716578</v>
       </c>
       <c r="T25" t="inlineStr">
         <is>
@@ -3891,13 +3891,13 @@
         <v>341</v>
       </c>
       <c r="Q26" t="n">
-        <v>13630</v>
+        <v>13625</v>
       </c>
       <c r="R26" t="n">
-        <v>346867</v>
+        <v>346709</v>
       </c>
       <c r="S26" t="n">
-        <v>671385</v>
+        <v>671007</v>
       </c>
       <c r="T26" t="inlineStr">
         <is>
@@ -3968,19 +3968,19 @@
         </is>
       </c>
       <c r="O27" t="n">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="P27" t="n">
         <v>913</v>
       </c>
       <c r="Q27" t="n">
-        <v>6372</v>
+        <v>6370</v>
       </c>
       <c r="R27" t="n">
-        <v>141779</v>
+        <v>141740</v>
       </c>
       <c r="S27" t="n">
-        <v>286346</v>
+        <v>286236</v>
       </c>
       <c r="T27" t="inlineStr">
         <is>
@@ -4055,7 +4055,7 @@
         </is>
       </c>
       <c r="O28" t="n">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="P28" t="n">
         <v>467</v>
@@ -4064,10 +4064,10 @@
         <v>10255</v>
       </c>
       <c r="R28" t="n">
-        <v>243545</v>
+        <v>243471</v>
       </c>
       <c r="S28" t="n">
-        <v>512957</v>
+        <v>512712</v>
       </c>
       <c r="T28" t="inlineStr">
         <is>
@@ -4138,19 +4138,19 @@
         </is>
       </c>
       <c r="O29" t="n">
-        <v>1818</v>
+        <v>1787</v>
       </c>
       <c r="P29" t="n">
-        <v>3222</v>
+        <v>3220</v>
       </c>
       <c r="Q29" t="n">
         <v>96</v>
       </c>
       <c r="R29" t="n">
-        <v>28326</v>
+        <v>28324</v>
       </c>
       <c r="S29" t="n">
-        <v>54312</v>
+        <v>54310</v>
       </c>
       <c r="T29" t="inlineStr">
         <is>
@@ -4227,13 +4227,13 @@
         <v>208</v>
       </c>
       <c r="Q30" t="n">
-        <v>14410</v>
+        <v>14408</v>
       </c>
       <c r="R30" t="n">
-        <v>539935</v>
+        <v>539696</v>
       </c>
       <c r="S30" t="n">
-        <v>912054</v>
+        <v>911525</v>
       </c>
       <c r="T30" t="inlineStr">
         <is>
@@ -4308,19 +4308,19 @@
         </is>
       </c>
       <c r="O31" t="n">
-        <v>4670</v>
+        <v>4695</v>
       </c>
       <c r="P31" t="n">
         <v>1370</v>
       </c>
       <c r="Q31" t="n">
-        <v>1433</v>
+        <v>1434</v>
       </c>
       <c r="R31" t="n">
-        <v>86319</v>
+        <v>86305</v>
       </c>
       <c r="S31" t="n">
-        <v>189276</v>
+        <v>189192</v>
       </c>
       <c r="T31" t="inlineStr">
         <is>
@@ -4391,19 +4391,19 @@
         </is>
       </c>
       <c r="O32" t="n">
-        <v>2934</v>
+        <v>2955</v>
       </c>
       <c r="P32" t="n">
-        <v>3152</v>
+        <v>3151</v>
       </c>
       <c r="Q32" t="n">
         <v>260</v>
       </c>
       <c r="R32" t="n">
-        <v>27840</v>
+        <v>27834</v>
       </c>
       <c r="S32" t="n">
-        <v>56606</v>
+        <v>56599</v>
       </c>
       <c r="T32" t="inlineStr">
         <is>
@@ -4478,19 +4478,19 @@
         </is>
       </c>
       <c r="O33" t="n">
-        <v>2829</v>
+        <v>2808</v>
       </c>
       <c r="P33" t="n">
-        <v>1551</v>
+        <v>1549</v>
       </c>
       <c r="Q33" t="n">
         <v>1150</v>
       </c>
       <c r="R33" t="n">
-        <v>79411</v>
+        <v>79400</v>
       </c>
       <c r="S33" t="n">
-        <v>165734</v>
+        <v>165669</v>
       </c>
       <c r="T33" t="inlineStr">
         <is>
@@ -4561,19 +4561,19 @@
         </is>
       </c>
       <c r="O34" t="n">
-        <v>8678</v>
+        <v>8693</v>
       </c>
       <c r="P34" t="n">
-        <v>3337</v>
+        <v>3332</v>
       </c>
       <c r="Q34" t="n">
         <v>187</v>
       </c>
       <c r="R34" t="n">
-        <v>27567</v>
+        <v>27564</v>
       </c>
       <c r="S34" t="n">
-        <v>51219</v>
+        <v>51207</v>
       </c>
       <c r="T34" t="inlineStr">
         <is>
@@ -4648,19 +4648,19 @@
         </is>
       </c>
       <c r="O35" t="n">
-        <v>3072</v>
+        <v>3091</v>
       </c>
       <c r="P35" t="n">
         <v>3029</v>
       </c>
       <c r="Q35" t="n">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="R35" t="n">
-        <v>29709</v>
+        <v>29705</v>
       </c>
       <c r="S35" t="n">
-        <v>61034</v>
+        <v>60992</v>
       </c>
       <c r="T35" t="inlineStr">
         <is>
@@ -4735,19 +4735,19 @@
         </is>
       </c>
       <c r="O36" t="n">
-        <v>3935</v>
+        <v>3951</v>
       </c>
       <c r="P36" t="n">
-        <v>2058</v>
+        <v>2057</v>
       </c>
       <c r="Q36" t="n">
         <v>472</v>
       </c>
       <c r="R36" t="n">
-        <v>55040</v>
+        <v>55031</v>
       </c>
       <c r="S36" t="n">
-        <v>114627</v>
+        <v>114589</v>
       </c>
       <c r="T36" t="inlineStr">
         <is>
@@ -4818,19 +4818,19 @@
         </is>
       </c>
       <c r="O37" t="n">
-        <v>4208</v>
+        <v>4177</v>
       </c>
       <c r="P37" t="n">
-        <v>2667</v>
+        <v>2663</v>
       </c>
       <c r="Q37" t="n">
         <v>186</v>
       </c>
       <c r="R37" t="n">
-        <v>42403</v>
+        <v>42394</v>
       </c>
       <c r="S37" t="n">
-        <v>76354</v>
+        <v>76339</v>
       </c>
       <c r="T37" t="inlineStr">
         <is>
@@ -4848,7 +4848,7 @@
         <v>55</v>
       </c>
       <c r="B38" t="n">
-        <v>6.48</v>
+        <v>6.49</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
@@ -4905,19 +4905,19 @@
         </is>
       </c>
       <c r="O38" t="n">
-        <v>7292</v>
+        <v>7210</v>
       </c>
       <c r="P38" t="n">
-        <v>5478</v>
+        <v>5477</v>
       </c>
       <c r="Q38" t="n">
         <v>14</v>
       </c>
       <c r="R38" t="n">
-        <v>6447</v>
+        <v>6444</v>
       </c>
       <c r="S38" t="n">
-        <v>17554</v>
+        <v>17540</v>
       </c>
       <c r="T38" t="inlineStr">
         <is>
@@ -4992,19 +4992,19 @@
         </is>
       </c>
       <c r="O39" t="n">
-        <v>10810</v>
+        <v>10791</v>
       </c>
       <c r="P39" t="n">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="Q39" t="n">
         <v>22</v>
       </c>
       <c r="R39" t="n">
-        <v>7313</v>
+        <v>7310</v>
       </c>
       <c r="S39" t="n">
-        <v>18718</v>
+        <v>18711</v>
       </c>
       <c r="T39" t="inlineStr">
         <is>
@@ -5079,19 +5079,19 @@
         </is>
       </c>
       <c r="O40" t="n">
-        <v>293</v>
+        <v>301</v>
       </c>
       <c r="P40" t="n">
         <v>716</v>
       </c>
       <c r="Q40" t="n">
-        <v>8828</v>
+        <v>8827</v>
       </c>
       <c r="R40" t="n">
-        <v>146223</v>
+        <v>146166</v>
       </c>
       <c r="S40" t="n">
-        <v>359562</v>
+        <v>359363</v>
       </c>
       <c r="T40" t="inlineStr">
         <is>
@@ -5166,19 +5166,19 @@
         </is>
       </c>
       <c r="O41" t="n">
-        <v>4371</v>
+        <v>4391</v>
       </c>
       <c r="P41" t="n">
-        <v>2488</v>
+        <v>2484</v>
       </c>
       <c r="Q41" t="n">
         <v>445</v>
       </c>
       <c r="R41" t="n">
-        <v>31566</v>
+        <v>31554</v>
       </c>
       <c r="S41" t="n">
-        <v>85700</v>
+        <v>85644</v>
       </c>
       <c r="T41" t="inlineStr">
         <is>
@@ -5253,7 +5253,7 @@
         </is>
       </c>
       <c r="O42" t="n">
-        <v>2443</v>
+        <v>2458</v>
       </c>
       <c r="P42" t="n">
         <v>484</v>
@@ -5262,10 +5262,10 @@
         <v>4174</v>
       </c>
       <c r="R42" t="n">
-        <v>260389</v>
+        <v>260340</v>
       </c>
       <c r="S42" t="n">
-        <v>500003</v>
+        <v>499813</v>
       </c>
       <c r="T42" t="inlineStr">
         <is>
@@ -5340,19 +5340,19 @@
         </is>
       </c>
       <c r="O43" t="n">
-        <v>1607</v>
+        <v>1610</v>
       </c>
       <c r="P43" t="n">
         <v>1136</v>
       </c>
       <c r="Q43" t="n">
-        <v>1944</v>
+        <v>1943</v>
       </c>
       <c r="R43" t="n">
-        <v>106085</v>
+        <v>106077</v>
       </c>
       <c r="S43" t="n">
-        <v>232604</v>
+        <v>232527</v>
       </c>
       <c r="T43" t="inlineStr">
         <is>
@@ -5427,19 +5427,19 @@
         </is>
       </c>
       <c r="O44" t="n">
-        <v>3617</v>
+        <v>3643</v>
       </c>
       <c r="P44" t="n">
-        <v>1376</v>
+        <v>1375</v>
       </c>
       <c r="Q44" t="n">
         <v>1281</v>
       </c>
       <c r="R44" t="n">
-        <v>100499</v>
+        <v>100497</v>
       </c>
       <c r="S44" t="n">
-        <v>188790</v>
+        <v>188739</v>
       </c>
       <c r="T44" t="inlineStr">
         <is>
@@ -5514,19 +5514,19 @@
         </is>
       </c>
       <c r="O45" t="n">
-        <v>5919</v>
+        <v>5915</v>
       </c>
       <c r="P45" t="n">
-        <v>2633</v>
+        <v>2632</v>
       </c>
       <c r="Q45" t="n">
         <v>199</v>
       </c>
       <c r="R45" t="n">
-        <v>31398</v>
+        <v>31399</v>
       </c>
       <c r="S45" t="n">
-        <v>78057</v>
+        <v>78040</v>
       </c>
       <c r="T45" t="inlineStr">
         <is>
@@ -5601,19 +5601,19 @@
         </is>
       </c>
       <c r="O46" t="n">
-        <v>6900</v>
+        <v>6887</v>
       </c>
       <c r="P46" t="n">
-        <v>1642</v>
+        <v>1640</v>
       </c>
       <c r="Q46" t="n">
         <v>360</v>
       </c>
       <c r="R46" t="n">
-        <v>81380</v>
+        <v>81363</v>
       </c>
       <c r="S46" t="n">
-        <v>153499</v>
+        <v>153401</v>
       </c>
       <c r="T46" t="inlineStr">
         <is>
@@ -5688,19 +5688,19 @@
         </is>
       </c>
       <c r="O47" t="n">
-        <v>2395</v>
+        <v>2396</v>
       </c>
       <c r="P47" t="n">
         <v>1229</v>
       </c>
       <c r="Q47" t="n">
-        <v>2064</v>
+        <v>2062</v>
       </c>
       <c r="R47" t="n">
-        <v>99966</v>
+        <v>99948</v>
       </c>
       <c r="S47" t="n">
-        <v>212934</v>
+        <v>212851</v>
       </c>
       <c r="T47" t="inlineStr">
         <is>
@@ -5775,19 +5775,19 @@
         </is>
       </c>
       <c r="O48" t="n">
-        <v>1563</v>
+        <v>1562</v>
       </c>
       <c r="P48" t="n">
         <v>2128</v>
       </c>
       <c r="Q48" t="n">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="R48" t="n">
-        <v>60538</v>
+        <v>60527</v>
       </c>
       <c r="S48" t="n">
-        <v>108707</v>
+        <v>108669</v>
       </c>
       <c r="T48" t="inlineStr">
         <is>
@@ -5862,19 +5862,19 @@
         </is>
       </c>
       <c r="O49" t="n">
-        <v>606</v>
+        <v>612</v>
       </c>
       <c r="P49" t="n">
         <v>638</v>
       </c>
       <c r="Q49" t="n">
-        <v>8558</v>
+        <v>8547</v>
       </c>
       <c r="R49" t="n">
-        <v>172117</v>
+        <v>171967</v>
       </c>
       <c r="S49" t="n">
-        <v>397130</v>
+        <v>396752</v>
       </c>
       <c r="T49" t="inlineStr">
         <is>
@@ -5949,19 +5949,19 @@
         </is>
       </c>
       <c r="O50" t="n">
-        <v>1883</v>
+        <v>1856</v>
       </c>
       <c r="P50" t="n">
         <v>1317</v>
       </c>
       <c r="Q50" t="n">
-        <v>1442</v>
+        <v>1443</v>
       </c>
       <c r="R50" t="n">
-        <v>80311</v>
+        <v>80291</v>
       </c>
       <c r="S50" t="n">
-        <v>197088</v>
+        <v>196984</v>
       </c>
       <c r="T50" t="inlineStr">
         <is>
@@ -6036,19 +6036,19 @@
         </is>
       </c>
       <c r="O51" t="n">
-        <v>2835</v>
+        <v>2813</v>
       </c>
       <c r="P51" t="n">
         <v>943</v>
       </c>
       <c r="Q51" t="n">
-        <v>1810</v>
+        <v>1811</v>
       </c>
       <c r="R51" t="n">
-        <v>131797</v>
+        <v>131780</v>
       </c>
       <c r="S51" t="n">
-        <v>277635</v>
+        <v>277596</v>
       </c>
       <c r="T51" t="inlineStr">
         <is>
@@ -6123,19 +6123,19 @@
         </is>
       </c>
       <c r="O52" t="n">
-        <v>8286</v>
+        <v>8302</v>
       </c>
       <c r="P52" t="n">
-        <v>6424</v>
+        <v>6418</v>
       </c>
       <c r="Q52" t="n">
         <v>14</v>
       </c>
       <c r="R52" t="n">
-        <v>3400</v>
+        <v>3398</v>
       </c>
       <c r="S52" t="n">
-        <v>11597</v>
+        <v>11592</v>
       </c>
       <c r="T52" t="inlineStr">
         <is>
@@ -6210,19 +6210,19 @@
         </is>
       </c>
       <c r="O53" t="n">
-        <v>1640</v>
+        <v>1627</v>
       </c>
       <c r="P53" t="n">
         <v>466</v>
       </c>
       <c r="Q53" t="n">
-        <v>4421</v>
+        <v>4418</v>
       </c>
       <c r="R53" t="n">
-        <v>247060</v>
+        <v>247023</v>
       </c>
       <c r="S53" t="n">
-        <v>514432</v>
+        <v>514273</v>
       </c>
       <c r="T53" t="inlineStr">
         <is>
@@ -6297,7 +6297,7 @@
         </is>
       </c>
       <c r="O54" t="n">
-        <v>644</v>
+        <v>649</v>
       </c>
       <c r="P54" t="n">
         <v>874</v>
@@ -6306,10 +6306,10 @@
         <v>2983</v>
       </c>
       <c r="R54" t="n">
-        <v>178910</v>
+        <v>178880</v>
       </c>
       <c r="S54" t="n">
-        <v>304988</v>
+        <v>304856</v>
       </c>
       <c r="T54" t="inlineStr">
         <is>
@@ -6384,19 +6384,19 @@
         </is>
       </c>
       <c r="O55" t="n">
-        <v>811</v>
+        <v>815</v>
       </c>
       <c r="P55" t="n">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="Q55" t="n">
-        <v>1297</v>
+        <v>1299</v>
       </c>
       <c r="R55" t="n">
-        <v>151505</v>
+        <v>151482</v>
       </c>
       <c r="S55" t="n">
-        <v>268113</v>
+        <v>268022</v>
       </c>
       <c r="T55" t="inlineStr">
         <is>
@@ -6471,19 +6471,19 @@
         </is>
       </c>
       <c r="O56" t="n">
-        <v>1482</v>
+        <v>1475</v>
       </c>
       <c r="P56" t="n">
-        <v>2187</v>
+        <v>2186</v>
       </c>
       <c r="Q56" t="n">
         <v>1490</v>
       </c>
       <c r="R56" t="n">
-        <v>53137</v>
+        <v>53125</v>
       </c>
       <c r="S56" t="n">
-        <v>104025</v>
+        <v>103982</v>
       </c>
       <c r="T56" t="inlineStr">
         <is>
@@ -6558,19 +6558,19 @@
         </is>
       </c>
       <c r="O57" t="n">
-        <v>3147</v>
+        <v>3160</v>
       </c>
       <c r="P57" t="n">
-        <v>3343</v>
+        <v>3340</v>
       </c>
       <c r="Q57" t="n">
         <v>276</v>
       </c>
       <c r="R57" t="n">
-        <v>15829</v>
+        <v>15826</v>
       </c>
       <c r="S57" t="n">
-        <v>51050</v>
+        <v>50995</v>
       </c>
       <c r="T57" t="inlineStr">
         <is>
@@ -6645,19 +6645,19 @@
         </is>
       </c>
       <c r="O58" t="n">
-        <v>2353</v>
+        <v>2369</v>
       </c>
       <c r="P58" t="n">
-        <v>2141</v>
+        <v>2139</v>
       </c>
       <c r="Q58" t="n">
-        <v>1064</v>
+        <v>1063</v>
       </c>
       <c r="R58" t="n">
-        <v>43447</v>
+        <v>43442</v>
       </c>
       <c r="S58" t="n">
-        <v>107867</v>
+        <v>107825</v>
       </c>
       <c r="T58" t="inlineStr">
         <is>
@@ -6732,19 +6732,19 @@
         </is>
       </c>
       <c r="O59" t="n">
-        <v>736</v>
+        <v>746</v>
       </c>
       <c r="P59" t="n">
-        <v>2856</v>
+        <v>2855</v>
       </c>
       <c r="Q59" t="n">
         <v>1015</v>
       </c>
       <c r="R59" t="n">
-        <v>34977</v>
+        <v>34966</v>
       </c>
       <c r="S59" t="n">
-        <v>68011</v>
+        <v>67980</v>
       </c>
       <c r="T59" t="inlineStr">
         <is>
@@ -6819,7 +6819,7 @@
         </is>
       </c>
       <c r="O60" t="n">
-        <v>4384</v>
+        <v>4391</v>
       </c>
       <c r="P60" t="n">
         <v>912</v>
@@ -6828,10 +6828,10 @@
         <v>1465</v>
       </c>
       <c r="R60" t="n">
-        <v>137897</v>
+        <v>137883</v>
       </c>
       <c r="S60" t="n">
-        <v>286467</v>
+        <v>286332</v>
       </c>
       <c r="T60" t="inlineStr">
         <is>
@@ -6906,19 +6906,19 @@
         </is>
       </c>
       <c r="O61" t="n">
-        <v>1152</v>
+        <v>1136</v>
       </c>
       <c r="P61" t="n">
-        <v>1726</v>
+        <v>1727</v>
       </c>
       <c r="Q61" t="n">
-        <v>2412</v>
+        <v>2406</v>
       </c>
       <c r="R61" t="n">
-        <v>64341</v>
+        <v>64290</v>
       </c>
       <c r="S61" t="n">
-        <v>142699</v>
+        <v>142532</v>
       </c>
       <c r="T61" t="inlineStr">
         <is>
@@ -6992,16 +6992,16 @@
         <v>678</v>
       </c>
       <c r="P62" t="n">
-        <v>2412</v>
+        <v>2408</v>
       </c>
       <c r="Q62" t="n">
         <v>1169</v>
       </c>
       <c r="R62" t="n">
-        <v>49316</v>
+        <v>49276</v>
       </c>
       <c r="S62" t="n">
-        <v>89790</v>
+        <v>89721</v>
       </c>
       <c r="T62" t="inlineStr">
         <is>
@@ -7072,19 +7072,19 @@
         </is>
       </c>
       <c r="O63" t="n">
-        <v>690</v>
+        <v>685</v>
       </c>
       <c r="P63" t="n">
-        <v>2903</v>
+        <v>2904</v>
       </c>
       <c r="Q63" t="n">
         <v>1119</v>
       </c>
       <c r="R63" t="n">
-        <v>36403</v>
+        <v>36376</v>
       </c>
       <c r="S63" t="n">
-        <v>65999</v>
+        <v>65950</v>
       </c>
       <c r="T63" t="inlineStr">
         <is>
@@ -7155,19 +7155,19 @@
         </is>
       </c>
       <c r="O64" t="n">
-        <v>5687</v>
+        <v>5686</v>
       </c>
       <c r="P64" t="n">
-        <v>5895</v>
+        <v>5894</v>
       </c>
       <c r="Q64" t="n">
         <v>5</v>
       </c>
       <c r="R64" t="n">
-        <v>7120</v>
+        <v>7118</v>
       </c>
       <c r="S64" t="n">
-        <v>14430</v>
+        <v>14426</v>
       </c>
       <c r="T64" t="inlineStr">
         <is>
@@ -7238,7 +7238,7 @@
         </is>
       </c>
       <c r="O65" t="n">
-        <v>3310</v>
+        <v>3274</v>
       </c>
       <c r="P65" t="n">
         <v>3419</v>
@@ -7247,10 +7247,10 @@
         <v>266</v>
       </c>
       <c r="R65" t="n">
-        <v>27409</v>
+        <v>27389</v>
       </c>
       <c r="S65" t="n">
-        <v>48733</v>
+        <v>48698</v>
       </c>
       <c r="T65" t="inlineStr">
         <is>
@@ -7331,13 +7331,13 @@
         <v>2561</v>
       </c>
       <c r="Q66" t="n">
-        <v>2406</v>
+        <v>2402</v>
       </c>
       <c r="R66" t="n">
-        <v>41792</v>
+        <v>41751</v>
       </c>
       <c r="S66" t="n">
-        <v>81831</v>
+        <v>81753</v>
       </c>
       <c r="T66" t="inlineStr">
         <is>
@@ -7412,7 +7412,7 @@
         </is>
       </c>
       <c r="O67" t="n">
-        <v>6215</v>
+        <v>6211</v>
       </c>
       <c r="P67" t="n">
         <v>3469</v>
@@ -7421,10 +7421,10 @@
         <v>189</v>
       </c>
       <c r="R67" t="n">
-        <v>23803</v>
+        <v>23782</v>
       </c>
       <c r="S67" t="n">
-        <v>47448</v>
+        <v>47407</v>
       </c>
       <c r="T67" t="inlineStr">
         <is>
@@ -7495,19 +7495,19 @@
         </is>
       </c>
       <c r="O68" t="n">
-        <v>1352</v>
+        <v>1364</v>
       </c>
       <c r="P68" t="n">
         <v>3209</v>
       </c>
       <c r="Q68" t="n">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="R68" t="n">
-        <v>32501</v>
+        <v>32467</v>
       </c>
       <c r="S68" t="n">
-        <v>54703</v>
+        <v>54656</v>
       </c>
       <c r="T68" t="inlineStr">
         <is>
@@ -7578,19 +7578,19 @@
         </is>
       </c>
       <c r="O69" t="n">
-        <v>6584</v>
+        <v>6582</v>
       </c>
       <c r="P69" t="n">
-        <v>4041</v>
+        <v>4042</v>
       </c>
       <c r="Q69" t="n">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="R69" t="n">
-        <v>19261</v>
+        <v>19238</v>
       </c>
       <c r="S69" t="n">
-        <v>35461</v>
+        <v>35432</v>
       </c>
       <c r="T69" t="inlineStr">
         <is>
@@ -7665,7 +7665,7 @@
         </is>
       </c>
       <c r="O70" t="n">
-        <v>5872</v>
+        <v>5874</v>
       </c>
       <c r="P70" t="n">
         <v>4352</v>
@@ -7674,10 +7674,10 @@
         <v>152</v>
       </c>
       <c r="R70" t="n">
-        <v>12190</v>
+        <v>12178</v>
       </c>
       <c r="S70" t="n">
-        <v>30355</v>
+        <v>30315</v>
       </c>
       <c r="T70" t="inlineStr">
         <is>
@@ -7752,19 +7752,19 @@
         </is>
       </c>
       <c r="O71" t="n">
-        <v>1383</v>
+        <v>1381</v>
       </c>
       <c r="P71" t="n">
-        <v>1546</v>
+        <v>1544</v>
       </c>
       <c r="Q71" t="n">
         <v>2416</v>
       </c>
       <c r="R71" t="n">
-        <v>92422</v>
+        <v>92388</v>
       </c>
       <c r="S71" t="n">
-        <v>166077</v>
+        <v>165966</v>
       </c>
       <c r="T71" t="inlineStr">
         <is>
@@ -7835,19 +7835,19 @@
         </is>
       </c>
       <c r="O72" t="n">
-        <v>1226</v>
+        <v>1238</v>
       </c>
       <c r="P72" t="n">
-        <v>3367</v>
+        <v>3366</v>
       </c>
       <c r="Q72" t="n">
         <v>182</v>
       </c>
       <c r="R72" t="n">
-        <v>28583</v>
+        <v>28571</v>
       </c>
       <c r="S72" t="n">
-        <v>50248</v>
+        <v>50228</v>
       </c>
       <c r="T72" t="inlineStr">
         <is>
@@ -7922,19 +7922,19 @@
         </is>
       </c>
       <c r="O73" t="n">
-        <v>2696</v>
+        <v>2703</v>
       </c>
       <c r="P73" t="n">
-        <v>3888</v>
+        <v>3885</v>
       </c>
       <c r="Q73" t="n">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="R73" t="n">
-        <v>17101</v>
+        <v>17091</v>
       </c>
       <c r="S73" t="n">
-        <v>38732</v>
+        <v>38696</v>
       </c>
       <c r="T73" t="inlineStr">
         <is>
@@ -8009,19 +8009,19 @@
         </is>
       </c>
       <c r="O74" t="n">
-        <v>1208</v>
+        <v>1207</v>
       </c>
       <c r="P74" t="n">
-        <v>1431</v>
+        <v>1430</v>
       </c>
       <c r="Q74" t="n">
         <v>3677</v>
       </c>
       <c r="R74" t="n">
-        <v>99506</v>
+        <v>99473</v>
       </c>
       <c r="S74" t="n">
-        <v>179117</v>
+        <v>179014</v>
       </c>
       <c r="T74" t="inlineStr">
         <is>
@@ -8096,19 +8096,19 @@
         </is>
       </c>
       <c r="O75" t="n">
-        <v>3583</v>
+        <v>3582</v>
       </c>
       <c r="P75" t="n">
-        <v>2073</v>
+        <v>2070</v>
       </c>
       <c r="Q75" t="n">
         <v>1136</v>
       </c>
       <c r="R75" t="n">
-        <v>67958</v>
+        <v>67937</v>
       </c>
       <c r="S75" t="n">
-        <v>113572</v>
+        <v>113509</v>
       </c>
       <c r="T75" t="inlineStr">
         <is>
@@ -8183,19 +8183,19 @@
         </is>
       </c>
       <c r="O76" t="n">
-        <v>1112</v>
+        <v>1097</v>
       </c>
       <c r="P76" t="n">
-        <v>3279</v>
+        <v>3277</v>
       </c>
       <c r="Q76" t="n">
-        <v>1138</v>
+        <v>1133</v>
       </c>
       <c r="R76" t="n">
-        <v>18575</v>
+        <v>18564</v>
       </c>
       <c r="S76" t="n">
-        <v>52494</v>
+        <v>52430</v>
       </c>
       <c r="T76" t="inlineStr">
         <is>
@@ -8270,19 +8270,19 @@
         </is>
       </c>
       <c r="O77" t="n">
-        <v>1678</v>
+        <v>1657</v>
       </c>
       <c r="P77" t="n">
-        <v>2750</v>
+        <v>2749</v>
       </c>
       <c r="Q77" t="n">
         <v>1065</v>
       </c>
       <c r="R77" t="n">
-        <v>39076</v>
+        <v>39067</v>
       </c>
       <c r="S77" t="n">
-        <v>72918</v>
+        <v>72879</v>
       </c>
       <c r="T77" t="inlineStr">
         <is>
@@ -8357,19 +8357,19 @@
         </is>
       </c>
       <c r="O78" t="n">
-        <v>1097</v>
+        <v>1101</v>
       </c>
       <c r="P78" t="n">
         <v>1419</v>
       </c>
       <c r="Q78" t="n">
-        <v>1892</v>
+        <v>1891</v>
       </c>
       <c r="R78" t="n">
-        <v>72806</v>
+        <v>72794</v>
       </c>
       <c r="S78" t="n">
-        <v>181226</v>
+        <v>181163</v>
       </c>
       <c r="T78" t="inlineStr">
         <is>
@@ -8444,7 +8444,7 @@
         </is>
       </c>
       <c r="O79" t="n">
-        <v>2413</v>
+        <v>2387</v>
       </c>
       <c r="P79" t="n">
         <v>1996</v>
@@ -8453,10 +8453,10 @@
         <v>1142</v>
       </c>
       <c r="R79" t="n">
-        <v>52934</v>
+        <v>52930</v>
       </c>
       <c r="S79" t="n">
-        <v>119221</v>
+        <v>119163</v>
       </c>
       <c r="T79" t="inlineStr">
         <is>
@@ -8531,19 +8531,19 @@
         </is>
       </c>
       <c r="O80" t="n">
-        <v>3008</v>
+        <v>3017</v>
       </c>
       <c r="P80" t="n">
-        <v>3252</v>
+        <v>3250</v>
       </c>
       <c r="Q80" t="n">
         <v>312</v>
       </c>
       <c r="R80" t="n">
-        <v>26024</v>
+        <v>26022</v>
       </c>
       <c r="S80" t="n">
-        <v>53150</v>
+        <v>53129</v>
       </c>
       <c r="T80" t="inlineStr">
         <is>
@@ -8618,19 +8618,19 @@
         </is>
       </c>
       <c r="O81" t="n">
-        <v>3705</v>
+        <v>3654</v>
       </c>
       <c r="P81" t="n">
-        <v>2885</v>
+        <v>2884</v>
       </c>
       <c r="Q81" t="n">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="R81" t="n">
-        <v>29835</v>
+        <v>29830</v>
       </c>
       <c r="S81" t="n">
-        <v>66966</v>
+        <v>66919</v>
       </c>
       <c r="T81" t="inlineStr">
         <is>

</xml_diff>